<commit_message>
Start implementing Single Times Log
</commit_message>
<xml_diff>
--- a/Assets/Logs/Template_Times Single and Total.xlsx
+++ b/Assets/Logs/Template_Times Single and Total.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t xml:space="preserve">task</t>
   </si>
@@ -28,10 +28,19 @@
     <t xml:space="preserve">item</t>
   </si>
   <si>
+    <t xml:space="preserve">time till score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">handling time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grabs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">varied grip</t>
+  </si>
+  <si>
     <t xml:space="preserve">time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grabs</t>
   </si>
   <si>
     <t xml:space="preserve">Task 1</t>
@@ -68,14 +77,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -135,8 +146,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -157,16 +172,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C79" activeCellId="0" sqref="C79"/>
+      <selection pane="topLeft" activeCell="F63" activeCellId="0" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.45"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.85"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.59"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -182,6 +199,12 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -191,9 +214,15 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="n">
+        <v>7.44</v>
+      </c>
+      <c r="D2" s="0" t="n">
         <v>6.44</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="E2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="b">
         <v>1</v>
       </c>
     </row>
@@ -205,10 +234,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="0" t="n">
+        <v>5.74</v>
+      </c>
+      <c r="D3" s="0" t="n">
         <v>4.74</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>1</v>
+      <c r="E3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -219,10 +254,16 @@
         <v>3</v>
       </c>
       <c r="C4" s="0" t="n">
+        <v>6.39</v>
+      </c>
+      <c r="D4" s="0" t="n">
         <v>5.39</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <v>3</v>
+      <c r="E4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -233,10 +274,16 @@
         <v>4</v>
       </c>
       <c r="C5" s="0" t="n">
+        <v>8.44</v>
+      </c>
+      <c r="D5" s="0" t="n">
         <v>7.44</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>2</v>
+      <c r="E5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -247,10 +294,16 @@
         <v>5</v>
       </c>
       <c r="C6" s="0" t="n">
+        <v>6.74</v>
+      </c>
+      <c r="D6" s="0" t="n">
         <v>5.74</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <v>2</v>
+      <c r="E6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -261,9 +314,15 @@
         <v>6</v>
       </c>
       <c r="C7" s="0" t="n">
+        <v>7.39</v>
+      </c>
+      <c r="D7" s="0" t="n">
         <v>6.39</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="b">
         <v>1</v>
       </c>
     </row>
@@ -275,10 +334,16 @@
         <v>7</v>
       </c>
       <c r="C8" s="0" t="n">
+        <v>9.44</v>
+      </c>
+      <c r="D8" s="0" t="n">
         <v>8.44</v>
       </c>
-      <c r="D8" s="0" t="n">
-        <v>3</v>
+      <c r="E8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F8" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -289,9 +354,15 @@
         <v>8</v>
       </c>
       <c r="C9" s="0" t="n">
+        <v>7.74</v>
+      </c>
+      <c r="D9" s="0" t="n">
         <v>6.74</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="E9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1" t="b">
         <v>1</v>
       </c>
     </row>
@@ -303,10 +374,16 @@
         <v>9</v>
       </c>
       <c r="C10" s="0" t="n">
+        <v>8.39</v>
+      </c>
+      <c r="D10" s="0" t="n">
         <v>7.39</v>
       </c>
-      <c r="D10" s="0" t="n">
-        <v>1</v>
+      <c r="E10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -317,10 +394,16 @@
         <v>10</v>
       </c>
       <c r="C11" s="0" t="n">
+        <v>10.44</v>
+      </c>
+      <c r="D11" s="0" t="n">
         <v>9.44</v>
       </c>
-      <c r="D11" s="0" t="n">
-        <v>4</v>
+      <c r="E11" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F11" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -331,10 +414,16 @@
         <v>11</v>
       </c>
       <c r="C12" s="0" t="n">
+        <v>8.74</v>
+      </c>
+      <c r="D12" s="0" t="n">
         <v>7.74</v>
       </c>
-      <c r="D12" s="0" t="n">
-        <v>4</v>
+      <c r="E12" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F12" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -345,10 +434,16 @@
         <v>12</v>
       </c>
       <c r="C13" s="0" t="n">
+        <v>9.39</v>
+      </c>
+      <c r="D13" s="0" t="n">
         <v>8.39</v>
       </c>
-      <c r="D13" s="0" t="n">
-        <v>1</v>
+      <c r="E13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -359,9 +454,15 @@
         <v>13</v>
       </c>
       <c r="C14" s="0" t="n">
+        <v>11.44</v>
+      </c>
+      <c r="D14" s="0" t="n">
         <v>10.44</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="E14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1" t="b">
         <v>1</v>
       </c>
     </row>
@@ -373,10 +474,16 @@
         <v>14</v>
       </c>
       <c r="C15" s="0" t="n">
+        <v>9.74</v>
+      </c>
+      <c r="D15" s="0" t="n">
         <v>8.74</v>
       </c>
-      <c r="D15" s="0" t="n">
-        <v>1</v>
+      <c r="E15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -387,10 +494,16 @@
         <v>15</v>
       </c>
       <c r="C16" s="0" t="n">
+        <v>10.39</v>
+      </c>
+      <c r="D16" s="0" t="n">
         <v>9.39</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="E16" s="0" t="n">
         <v>7</v>
+      </c>
+      <c r="F16" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -401,9 +514,15 @@
         <v>1</v>
       </c>
       <c r="C17" s="0" t="n">
+        <v>4.54</v>
+      </c>
+      <c r="D17" s="0" t="n">
         <v>3.54</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="E17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1" t="b">
         <v>1</v>
       </c>
     </row>
@@ -415,9 +534,15 @@
         <v>2</v>
       </c>
       <c r="C18" s="0" t="n">
+        <v>7.48</v>
+      </c>
+      <c r="D18" s="0" t="n">
         <v>6.48</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="E18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1" t="b">
         <v>1</v>
       </c>
     </row>
@@ -429,10 +554,16 @@
         <v>3</v>
       </c>
       <c r="C19" s="0" t="n">
+        <v>5.89</v>
+      </c>
+      <c r="D19" s="0" t="n">
         <v>4.89</v>
       </c>
-      <c r="D19" s="0" t="n">
-        <v>2</v>
+      <c r="E19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F19" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -443,10 +574,16 @@
         <v>2</v>
       </c>
       <c r="C20" s="0" t="n">
+        <v>8.44</v>
+      </c>
+      <c r="D20" s="0" t="n">
         <v>7.44</v>
       </c>
-      <c r="D20" s="0" t="n">
-        <v>2</v>
+      <c r="E20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -457,10 +594,16 @@
         <v>3</v>
       </c>
       <c r="C21" s="0" t="n">
+        <v>6.74</v>
+      </c>
+      <c r="D21" s="0" t="n">
         <v>5.74</v>
       </c>
-      <c r="D21" s="0" t="n">
-        <v>2</v>
+      <c r="E21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -471,10 +614,16 @@
         <v>4</v>
       </c>
       <c r="C22" s="0" t="n">
+        <v>7.39</v>
+      </c>
+      <c r="D22" s="0" t="n">
         <v>6.39</v>
       </c>
-      <c r="D22" s="0" t="n">
-        <v>4</v>
+      <c r="E22" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F22" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -485,10 +634,16 @@
         <v>5</v>
       </c>
       <c r="C23" s="0" t="n">
+        <v>9.44</v>
+      </c>
+      <c r="D23" s="0" t="n">
         <v>8.44</v>
       </c>
-      <c r="D23" s="0" t="n">
-        <v>3</v>
+      <c r="E23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F23" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -499,10 +654,16 @@
         <v>6</v>
       </c>
       <c r="C24" s="0" t="n">
+        <v>7.74</v>
+      </c>
+      <c r="D24" s="0" t="n">
         <v>6.74</v>
       </c>
-      <c r="D24" s="0" t="n">
-        <v>3</v>
+      <c r="E24" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F24" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -513,10 +674,16 @@
         <v>7</v>
       </c>
       <c r="C25" s="0" t="n">
+        <v>8.39</v>
+      </c>
+      <c r="D25" s="0" t="n">
         <v>7.39</v>
       </c>
-      <c r="D25" s="0" t="n">
-        <v>2</v>
+      <c r="E25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F25" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -527,10 +694,16 @@
         <v>8</v>
       </c>
       <c r="C26" s="0" t="n">
+        <v>10.44</v>
+      </c>
+      <c r="D26" s="0" t="n">
         <v>9.44</v>
       </c>
-      <c r="D26" s="0" t="n">
-        <v>4</v>
+      <c r="E26" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F26" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -541,10 +714,16 @@
         <v>9</v>
       </c>
       <c r="C27" s="0" t="n">
+        <v>8.74</v>
+      </c>
+      <c r="D27" s="0" t="n">
         <v>7.74</v>
       </c>
-      <c r="D27" s="0" t="n">
-        <v>2</v>
+      <c r="E27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F27" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -555,10 +734,16 @@
         <v>10</v>
       </c>
       <c r="C28" s="0" t="n">
+        <v>9.39</v>
+      </c>
+      <c r="D28" s="0" t="n">
         <v>8.39</v>
       </c>
-      <c r="D28" s="0" t="n">
-        <v>2</v>
+      <c r="E28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F28" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -569,10 +754,16 @@
         <v>11</v>
       </c>
       <c r="C29" s="0" t="n">
+        <v>11.44</v>
+      </c>
+      <c r="D29" s="0" t="n">
         <v>10.44</v>
       </c>
-      <c r="D29" s="0" t="n">
+      <c r="E29" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="F29" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -583,10 +774,16 @@
         <v>12</v>
       </c>
       <c r="C30" s="0" t="n">
+        <v>9.74</v>
+      </c>
+      <c r="D30" s="0" t="n">
         <v>8.74</v>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="E30" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="F30" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -597,10 +794,16 @@
         <v>13</v>
       </c>
       <c r="C31" s="0" t="n">
+        <v>10.39</v>
+      </c>
+      <c r="D31" s="0" t="n">
         <v>9.39</v>
       </c>
-      <c r="D31" s="0" t="n">
-        <v>2</v>
+      <c r="E31" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F31" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -611,10 +814,16 @@
         <v>14</v>
       </c>
       <c r="C32" s="0" t="n">
+        <v>12.44</v>
+      </c>
+      <c r="D32" s="0" t="n">
         <v>11.44</v>
       </c>
-      <c r="D32" s="0" t="n">
-        <v>2</v>
+      <c r="E32" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F32" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -625,10 +834,16 @@
         <v>15</v>
       </c>
       <c r="C33" s="0" t="n">
+        <v>10.74</v>
+      </c>
+      <c r="D33" s="0" t="n">
         <v>9.74</v>
       </c>
-      <c r="D33" s="0" t="n">
-        <v>2</v>
+      <c r="E33" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F33" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -639,9 +854,15 @@
         <v>1</v>
       </c>
       <c r="C34" s="0" t="n">
+        <v>6.98</v>
+      </c>
+      <c r="D34" s="0" t="n">
         <v>5.98</v>
       </c>
-      <c r="D34" s="0" t="n">
+      <c r="E34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F34" s="1" t="b">
         <v>1</v>
       </c>
     </row>
@@ -653,10 +874,16 @@
         <v>2</v>
       </c>
       <c r="C35" s="0" t="n">
+        <v>5.54</v>
+      </c>
+      <c r="D35" s="0" t="n">
         <v>4.54</v>
       </c>
-      <c r="D35" s="0" t="n">
-        <v>2</v>
+      <c r="E35" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F35" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -667,10 +894,16 @@
         <v>3</v>
       </c>
       <c r="C36" s="0" t="n">
+        <v>8.48</v>
+      </c>
+      <c r="D36" s="0" t="n">
         <v>7.48</v>
       </c>
-      <c r="D36" s="0" t="n">
-        <v>2</v>
+      <c r="E36" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F36" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -681,10 +914,16 @@
         <v>4</v>
       </c>
       <c r="C37" s="0" t="n">
+        <v>6.89</v>
+      </c>
+      <c r="D37" s="0" t="n">
         <v>5.89</v>
       </c>
-      <c r="D37" s="0" t="n">
-        <v>3</v>
+      <c r="E37" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F37" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -695,9 +934,15 @@
         <v>3</v>
       </c>
       <c r="C38" s="0" t="n">
+        <v>9.44</v>
+      </c>
+      <c r="D38" s="0" t="n">
         <v>8.44</v>
       </c>
-      <c r="D38" s="0" t="n">
+      <c r="E38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F38" s="1" t="b">
         <v>1</v>
       </c>
     </row>
@@ -709,10 +954,16 @@
         <v>4</v>
       </c>
       <c r="C39" s="0" t="n">
+        <v>7.74</v>
+      </c>
+      <c r="D39" s="0" t="n">
         <v>6.74</v>
       </c>
-      <c r="D39" s="0" t="n">
-        <v>3</v>
+      <c r="E39" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F39" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -723,10 +974,16 @@
         <v>5</v>
       </c>
       <c r="C40" s="0" t="n">
+        <v>8.39</v>
+      </c>
+      <c r="D40" s="0" t="n">
         <v>7.39</v>
       </c>
-      <c r="D40" s="0" t="n">
-        <v>1</v>
+      <c r="E40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F40" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -737,9 +994,15 @@
         <v>6</v>
       </c>
       <c r="C41" s="0" t="n">
+        <v>10.44</v>
+      </c>
+      <c r="D41" s="0" t="n">
         <v>9.44</v>
       </c>
-      <c r="D41" s="0" t="n">
+      <c r="E41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F41" s="1" t="b">
         <v>1</v>
       </c>
     </row>
@@ -751,10 +1014,16 @@
         <v>7</v>
       </c>
       <c r="C42" s="0" t="n">
+        <v>8.74</v>
+      </c>
+      <c r="D42" s="0" t="n">
         <v>7.74</v>
       </c>
-      <c r="D42" s="0" t="n">
-        <v>1</v>
+      <c r="E42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -765,10 +1034,16 @@
         <v>8</v>
       </c>
       <c r="C43" s="0" t="n">
+        <v>9.39</v>
+      </c>
+      <c r="D43" s="0" t="n">
         <v>8.39</v>
       </c>
-      <c r="D43" s="0" t="n">
-        <v>3</v>
+      <c r="E43" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F43" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -779,9 +1054,15 @@
         <v>9</v>
       </c>
       <c r="C44" s="0" t="n">
+        <v>11.44</v>
+      </c>
+      <c r="D44" s="0" t="n">
         <v>10.44</v>
       </c>
-      <c r="D44" s="0" t="n">
+      <c r="E44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F44" s="1" t="b">
         <v>1</v>
       </c>
     </row>
@@ -793,10 +1074,16 @@
         <v>10</v>
       </c>
       <c r="C45" s="0" t="n">
+        <v>9.74</v>
+      </c>
+      <c r="D45" s="0" t="n">
         <v>8.74</v>
       </c>
-      <c r="D45" s="0" t="n">
-        <v>3</v>
+      <c r="E45" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F45" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -807,10 +1094,16 @@
         <v>11</v>
       </c>
       <c r="C46" s="0" t="n">
+        <v>10.39</v>
+      </c>
+      <c r="D46" s="0" t="n">
         <v>9.39</v>
       </c>
-      <c r="D46" s="0" t="n">
-        <v>1</v>
+      <c r="E46" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F46" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -821,9 +1114,15 @@
         <v>12</v>
       </c>
       <c r="C47" s="0" t="n">
+        <v>12.44</v>
+      </c>
+      <c r="D47" s="0" t="n">
         <v>11.44</v>
       </c>
-      <c r="D47" s="0" t="n">
+      <c r="E47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F47" s="1" t="b">
         <v>1</v>
       </c>
     </row>
@@ -835,10 +1134,16 @@
         <v>13</v>
       </c>
       <c r="C48" s="0" t="n">
+        <v>7.98</v>
+      </c>
+      <c r="D48" s="0" t="n">
         <v>6.98</v>
       </c>
-      <c r="D48" s="0" t="n">
-        <v>2</v>
+      <c r="E48" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F48" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -849,10 +1154,16 @@
         <v>14</v>
       </c>
       <c r="C49" s="0" t="n">
+        <v>6.54</v>
+      </c>
+      <c r="D49" s="0" t="n">
         <v>5.54</v>
       </c>
-      <c r="D49" s="0" t="n">
-        <v>3</v>
+      <c r="E49" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F49" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -863,10 +1174,16 @@
         <v>15</v>
       </c>
       <c r="C50" s="0" t="n">
+        <v>7.98</v>
+      </c>
+      <c r="D50" s="0" t="n">
         <v>6.98</v>
       </c>
-      <c r="D50" s="0" t="n">
-        <v>2</v>
+      <c r="E50" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F50" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -877,10 +1194,16 @@
         <v>1</v>
       </c>
       <c r="C51" s="0" t="n">
+        <v>4.54</v>
+      </c>
+      <c r="D51" s="0" t="n">
         <v>3.54</v>
       </c>
-      <c r="D51" s="0" t="n">
-        <v>1</v>
+      <c r="E51" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F51" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -891,9 +1214,15 @@
         <v>2</v>
       </c>
       <c r="C52" s="0" t="n">
+        <v>5.95</v>
+      </c>
+      <c r="D52" s="0" t="n">
         <v>4.95</v>
       </c>
-      <c r="D52" s="0" t="n">
+      <c r="E52" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F52" s="1" t="b">
         <v>1</v>
       </c>
     </row>
@@ -905,10 +1234,16 @@
         <v>3</v>
       </c>
       <c r="C53" s="0" t="n">
+        <v>7.36</v>
+      </c>
+      <c r="D53" s="0" t="n">
         <v>6.36</v>
       </c>
-      <c r="D53" s="0" t="n">
-        <v>2</v>
+      <c r="E53" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F53" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -919,9 +1254,15 @@
         <v>4</v>
       </c>
       <c r="C54" s="0" t="n">
+        <v>3.84</v>
+      </c>
+      <c r="D54" s="0" t="n">
         <v>2.84</v>
       </c>
-      <c r="D54" s="0" t="n">
+      <c r="E54" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F54" s="1" t="b">
         <v>1</v>
       </c>
     </row>
@@ -933,10 +1274,16 @@
         <v>5</v>
       </c>
       <c r="C55" s="0" t="n">
+        <v>5.54</v>
+      </c>
+      <c r="D55" s="0" t="n">
         <v>4.54</v>
       </c>
-      <c r="D55" s="0" t="n">
-        <v>2</v>
+      <c r="E55" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F55" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -947,10 +1294,16 @@
         <v>6</v>
       </c>
       <c r="C56" s="0" t="n">
+        <v>6.95</v>
+      </c>
+      <c r="D56" s="0" t="n">
         <v>5.95</v>
       </c>
-      <c r="D56" s="0" t="n">
-        <v>2</v>
+      <c r="E56" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F56" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -961,10 +1314,16 @@
         <v>7</v>
       </c>
       <c r="C57" s="0" t="n">
+        <v>8.36</v>
+      </c>
+      <c r="D57" s="0" t="n">
         <v>7.36</v>
       </c>
-      <c r="D57" s="0" t="n">
-        <v>3</v>
+      <c r="E57" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F57" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -975,10 +1334,16 @@
         <v>8</v>
       </c>
       <c r="C58" s="0" t="n">
+        <v>4.84</v>
+      </c>
+      <c r="D58" s="0" t="n">
         <v>3.84</v>
       </c>
-      <c r="D58" s="0" t="n">
-        <v>2</v>
+      <c r="E58" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F58" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -989,10 +1354,16 @@
         <v>9</v>
       </c>
       <c r="C59" s="0" t="n">
+        <v>6.54</v>
+      </c>
+      <c r="D59" s="0" t="n">
         <v>5.54</v>
       </c>
-      <c r="D59" s="0" t="n">
-        <v>3</v>
+      <c r="E59" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F59" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1003,10 +1374,16 @@
         <v>10</v>
       </c>
       <c r="C60" s="0" t="n">
+        <v>7.95</v>
+      </c>
+      <c r="D60" s="0" t="n">
         <v>6.95</v>
       </c>
-      <c r="D60" s="0" t="n">
-        <v>3</v>
+      <c r="E60" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F60" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1017,10 +1394,16 @@
         <v>11</v>
       </c>
       <c r="C61" s="0" t="n">
+        <v>9.36</v>
+      </c>
+      <c r="D61" s="0" t="n">
         <v>8.36</v>
       </c>
-      <c r="D61" s="0" t="n">
-        <v>4</v>
+      <c r="E61" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F61" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1031,10 +1414,16 @@
         <v>12</v>
       </c>
       <c r="C62" s="0" t="n">
+        <v>5.84</v>
+      </c>
+      <c r="D62" s="0" t="n">
         <v>4.84</v>
       </c>
-      <c r="D62" s="0" t="n">
-        <v>3</v>
+      <c r="E62" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F62" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1045,10 +1434,16 @@
         <v>13</v>
       </c>
       <c r="C63" s="0" t="n">
+        <v>7.54</v>
+      </c>
+      <c r="D63" s="0" t="n">
         <v>6.54</v>
       </c>
-      <c r="D63" s="0" t="n">
-        <v>4</v>
+      <c r="E63" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F63" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1059,10 +1454,16 @@
         <v>14</v>
       </c>
       <c r="C64" s="0" t="n">
+        <v>8.95</v>
+      </c>
+      <c r="D64" s="0" t="n">
         <v>7.95</v>
       </c>
-      <c r="D64" s="0" t="n">
-        <v>4</v>
+      <c r="E64" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F64" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1073,10 +1474,16 @@
         <v>15</v>
       </c>
       <c r="C65" s="0" t="n">
+        <v>10.36</v>
+      </c>
+      <c r="D65" s="0" t="n">
         <v>9.36</v>
       </c>
-      <c r="D65" s="0" t="n">
+      <c r="E65" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="F65" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1084,12 +1491,12 @@
         <v>0</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>253</v>
@@ -1097,7 +1504,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>252</v>
@@ -1105,7 +1512,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>256</v>
@@ -1113,7 +1520,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>251</v>
@@ -1121,7 +1528,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B74" s="0" t="n">
         <f aca="false">SUM(B70:B73)</f>
@@ -1130,43 +1537,43 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B75" s="0" t="n">
-        <f aca="false">SUM(C2:C16)</f>
+        <f aca="false">SUM(D2:D16)</f>
         <v>112.85</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B76" s="0" t="n">
-        <f aca="false">SUM(C17:C33)</f>
+        <f aca="false">SUM(D17:D33)</f>
         <v>132.37</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B77" s="0" t="n">
-        <f aca="false">SUM(C34:C50)</f>
+        <f aca="false">SUM(D34:D50)</f>
         <v>131.54</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B78" s="0" t="n">
-        <f aca="false">SUM(C51:C65)</f>
+        <f aca="false">SUM(D51:D65)</f>
         <v>88.92</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B79" s="0" t="n">
         <f aca="false">SUM(B75:B78)</f>

</xml_diff>